<commit_message>
Updates to xw_get_named_range function. Tests.
Updated xw_get_named_range() function to use the .refers_to_range
property from workbook.names[range_name]. Removes confusign and
non-foolproof regex from the function. Throws an error if any of the
names have a #REF! error in Excel. Will eventually need to clean that up
to have better error handling.
Updated datum_excel_tests workbook in prep for unit test framework.
Updated .gitignore to ignore NX files in tests dir
</commit_message>
<xml_diff>
--- a/tests/datum_excel_tests.xlsx
+++ b/tests/datum_excel_tests.xlsx
@@ -1,42 +1,83 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20384"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\blair\datum\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frandeen\Documents\datum\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D986674-3A8C-4145-B384-57F5D0E9B280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08302301-BE85-4FF5-9839-DB31766307E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="96" windowWidth="11580" windowHeight="13584" xr2:uid="{4E3D2296-B548-4056-9C4B-8EF4E130383B}"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="11580" windowHeight="13590" xr2:uid="{4E3D2296-B548-4056-9C4B-8EF4E130383B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Gearbox Tests" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Date_range">Sheet1!$A$3</definedName>
-    <definedName name="float_range">Sheet1!$A$2</definedName>
-    <definedName name="Test_Range_1">Sheet1!$A$1</definedName>
+    <definedName name="AIR_NUT">'Gearbox Tests'!$C$9</definedName>
+    <definedName name="Date_range">'Gearbox Tests'!$A$3</definedName>
+    <definedName name="DIPSTICK">'Gearbox Tests'!$C$8</definedName>
+    <definedName name="FASTENERS.mass">'Gearbox Tests'!$C$6</definedName>
+    <definedName name="float_range">'Gearbox Tests'!$A$2</definedName>
+    <definedName name="GEARS.mass">'Gearbox Tests'!$C$7</definedName>
+    <definedName name="HOUSING.mass">'Gearbox Tests'!$C$5</definedName>
+    <definedName name="SHAFT_CENTERS">'Gearbox Tests'!$C$10</definedName>
+    <definedName name="SURFACE_PAINTED.area">'Gearbox Tests'!$C$4</definedName>
+    <definedName name="Test_Range_1">'Gearbox Tests'!$A$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+  <si>
+    <t>Because spreadsheets need dark mode too!</t>
+  </si>
+  <si>
+    <t>Gearbox parameters</t>
+  </si>
+  <si>
+    <t>SURFACE_PAINTED.area</t>
+  </si>
+  <si>
+    <t>HOUSING.mass</t>
+  </si>
+  <si>
+    <t>FASTENERS.mass</t>
+  </si>
+  <si>
+    <t>GEARS.mass</t>
+  </si>
+  <si>
+    <t>DIPSTICK</t>
+  </si>
+  <si>
+    <t>AIR NUT</t>
+  </si>
+  <si>
+    <t>SHAFT CENTERS</t>
+  </si>
+  <si>
+    <t>mm2</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>deg</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -401,31 +442,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54907CF9-C14B-4766-B22F-13A5988C480B}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>44642</v>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
unit test improvements for xlpnr
</commit_message>
<xml_diff>
--- a/tests/datum_excel_tests.xlsx
+++ b/tests/datum_excel_tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blair\datum\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A22FDA55-7BF2-4448-B5CE-1F379F04E524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C44D973-3024-4564-9511-2DAD7C5A4B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="3000" windowWidth="17280" windowHeight="10008" xr2:uid="{4E3D2296-B548-4056-9C4B-8EF4E130383B}"/>
+    <workbookView xWindow="468" yWindow="924" windowWidth="5952" windowHeight="9180" xr2:uid="{4E3D2296-B548-4056-9C4B-8EF4E130383B}"/>
   </bookViews>
   <sheets>
     <sheet name="Other Tests" sheetId="3" r:id="rId1"/>
@@ -24,10 +24,14 @@
     <definedName name="float_range">'Gearbox Tests'!$A$2</definedName>
     <definedName name="GEARS.mass">'Gearbox Tests'!$C$7</definedName>
     <definedName name="HOUSING.mass">'Gearbox Tests'!$C$5</definedName>
-    <definedName name="missing_ref">'Other Tests'!$C$1</definedName>
+    <definedName name="missing_ref">'Other Tests'!#REF!</definedName>
     <definedName name="SHAFT_CENTERS">'Gearbox Tests'!$C$10</definedName>
     <definedName name="SURFACE_PAINTED.area">'Gearbox Tests'!$C$4</definedName>
+    <definedName name="Test_Date">'Other Tests'!$B$5</definedName>
+    <definedName name="Test_Float">'Other Tests'!$B$4</definedName>
+    <definedName name="Test_Int">'Other Tests'!$B$2</definedName>
     <definedName name="Test_Range_1">'Gearbox Tests'!$A$1</definedName>
+    <definedName name="Test_Str">'Other Tests'!$B$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Because spreadsheets need dark mode too!</t>
   </si>
@@ -90,7 +94,22 @@
     <t>mm</t>
   </si>
   <si>
-    <t>Range with missing reference</t>
+    <t>Kivo is a dork</t>
+  </si>
+  <si>
+    <t>Test Int</t>
+  </si>
+  <si>
+    <t>Test Str</t>
+  </si>
+  <si>
+    <t>Test Float</t>
+  </si>
+  <si>
+    <t>Test Date</t>
+  </si>
+  <si>
+    <t>TEST VALUES -- DO NOT MODIFY</t>
   </si>
 </sst>
 </file>
@@ -113,7 +132,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -123,6 +142,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -139,10 +164,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F223915-F445-4D32-BCC2-8C7735AB3DA4}">
-  <dimension ref="B1:C1"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -470,16 +498,48 @@
     <col min="3" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="3"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="1" t="e">
-        <f>#REF!*5</f>
-        <v>#REF!</v>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3.1415190000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2">
+        <v>44682</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactoring of XLPNR, add undo functionality
Split up the `update_named_ranges` function in xlpnr into slightly more
logical blocks. This area still needs some work, but the code is a bit
clearer and more functional than it was. I don't know that it's worth
trying too hard to refactor further until I give measurement values
their own class (rather than just floats as they are now).

Added undo functionality, so that `update_named_ranges` returns a
dictionary of the ranges that were updated and the previous
values. This allows the user to undo an update command immediately after
it was executed, since ctrl+z functionality within Excel is no help
here.
</commit_message>
<xml_diff>
--- a/tests/datum_excel_tests.xlsx
+++ b/tests/datum_excel_tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blair\datum\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C44D973-3024-4564-9511-2DAD7C5A4B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9395B8-899A-4BE8-87F5-B449082E940B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="468" yWindow="924" windowWidth="5952" windowHeight="9180" xr2:uid="{4E3D2296-B548-4056-9C4B-8EF4E130383B}"/>
+    <workbookView xWindow="3384" yWindow="3384" windowWidth="7500" windowHeight="9180" firstSheet="1" activeTab="1" xr2:uid="{4E3D2296-B548-4056-9C4B-8EF4E130383B}"/>
   </bookViews>
   <sheets>
     <sheet name="Other Tests" sheetId="3" r:id="rId1"/>
@@ -487,7 +487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F223915-F445-4D32-BCC2-8C7735AB3DA4}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -549,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54907CF9-C14B-4766-B22F-13A5988C480B}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -575,6 +575,9 @@
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
       <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
@@ -583,6 +586,9 @@
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C5" s="1">
+        <v>2</v>
+      </c>
       <c r="D5" s="1" t="s">
         <v>10</v>
       </c>
@@ -591,6 +597,9 @@
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="C6" s="1">
+        <v>4</v>
+      </c>
       <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
@@ -599,6 +608,9 @@
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C7" s="1">
+        <v>5</v>
+      </c>
       <c r="D7" s="1" t="s">
         <v>10</v>
       </c>
@@ -607,6 +619,9 @@
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="C8" s="1">
+        <v>3</v>
+      </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
       </c>
@@ -615,10 +630,16 @@
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="C9" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="C10" s="1">
+        <v>7</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
add unit test for update_named_ranges
</commit_message>
<xml_diff>
--- a/tests/datum_excel_tests.xlsx
+++ b/tests/datum_excel_tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blair\datum\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9395B8-899A-4BE8-87F5-B449082E940B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E7343D3-3049-42F5-B1DA-707205E853F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3384" yWindow="3384" windowWidth="7500" windowHeight="9180" firstSheet="1" activeTab="1" xr2:uid="{4E3D2296-B548-4056-9C4B-8EF4E130383B}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="10008" firstSheet="1" activeTab="1" xr2:uid="{4E3D2296-B548-4056-9C4B-8EF4E130383B}"/>
   </bookViews>
   <sheets>
     <sheet name="Other Tests" sheetId="3" r:id="rId1"/>
@@ -576,7 +576,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="1">
-        <v>3</v>
+        <v>731851.44965614588</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>9</v>
@@ -587,7 +587,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="1">
-        <v>2</v>
+        <v>128850.48535948661</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>10</v>
@@ -598,7 +598,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="1">
-        <v>4</v>
+        <v>3802.9230326870379</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>10</v>
@@ -609,7 +609,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="1">
-        <v>5</v>
+        <v>54455.593060061852</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>10</v>
@@ -620,7 +620,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="1">
-        <v>3</v>
+        <v>90</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Clean up of XLPNR
Simplified the main XLPNR algorithm by splitting off functions for
getting measurements & names from JSON and Excel, respectively. Both of
the above functions return dicts of names and values, and only the
common names/values are written to Excel.

Minor updates to unit tests. Unit tests not yet comprehensive, needing
to write tests for get_json_measurement_names and
get_workbook_range_names. More comprehensive testing for
update_named_ranges and write_named_ranges will be needed. Some
refactoring needed. Cleaner than it was.
</commit_message>
<xml_diff>
--- a/tests/datum_excel_tests.xlsx
+++ b/tests/datum_excel_tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blair\datum\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E7343D3-3049-42F5-B1DA-707205E853F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BCAB3E8-38C7-4C61-8ADE-549A21428737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="10008" firstSheet="1" activeTab="1" xr2:uid="{4E3D2296-B548-4056-9C4B-8EF4E130383B}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="10008" firstSheet="1" activeTab="1" xr2:uid="{4E3D2296-B548-4056-9C4B-8EF4E130383B}"/>
   </bookViews>
   <sheets>
     <sheet name="Other Tests" sheetId="3" r:id="rId1"/>
@@ -587,7 +587,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="1">
-        <v>128850.48535948661</v>
+        <v>128.85048535948661</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>10</v>
@@ -598,7 +598,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="1">
-        <v>3802.9230326870379</v>
+        <v>3.8029230326870378</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>10</v>
@@ -609,7 +609,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="1">
-        <v>54455.593060061852</v>
+        <v>54.455593060061851</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
increase unit test coverage.
</commit_message>
<xml_diff>
--- a/tests/datum_excel_tests.xlsx
+++ b/tests/datum_excel_tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blair\datum\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BCAB3E8-38C7-4C61-8ADE-549A21428737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B6907A-4214-4508-AD0C-D407DE585DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="10008" firstSheet="1" activeTab="1" xr2:uid="{4E3D2296-B548-4056-9C4B-8EF4E130383B}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="10008" firstSheet="1" activeTab="1" xr2:uid="{4E3D2296-B548-4056-9C4B-8EF4E130383B}"/>
   </bookViews>
   <sheets>
     <sheet name="Other Tests" sheetId="3" r:id="rId1"/>
@@ -576,7 +576,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="1">
-        <v>731851.44965614588</v>
+        <v>700000</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>9</v>

</xml_diff>